<commit_message>
Manufacturing files for Rev A
</commit_message>
<xml_diff>
--- a/bom.xlsx
+++ b/bom.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rich\development\UWaterloo\dsp_pid\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rich\development\UWaterloo\dsp_pid.git\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="10380"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="24000" windowHeight="10380"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="193">
   <si>
     <t>QTY</t>
   </si>
@@ -401,9 +401,6 @@
     <t>OPA1679IPWR</t>
   </si>
   <si>
-    <t>OPA1679IPWR-ND</t>
-  </si>
-  <si>
     <t>U3,</t>
   </si>
   <si>
@@ -473,9 +470,6 @@
     <t>XP1001000-05R</t>
   </si>
   <si>
-    <t>1829-1000-ND</t>
-  </si>
-  <si>
     <t>U7,</t>
   </si>
   <si>
@@ -531,13 +525,91 @@
   </si>
   <si>
     <t>535-9918-1-ND</t>
+  </si>
+  <si>
+    <t>100N</t>
+  </si>
+  <si>
+    <t>1276-1061-1-ND</t>
+  </si>
+  <si>
+    <t>1276-1926-1-ND</t>
+  </si>
+  <si>
+    <t>1276-1019-1-ND</t>
+  </si>
+  <si>
+    <t>399-8979-1-ND</t>
+  </si>
+  <si>
+    <t>1276-2092-1-ND</t>
+  </si>
+  <si>
+    <t>399-1089-1-ND</t>
+  </si>
+  <si>
+    <t>490-3282-1-ND</t>
+  </si>
+  <si>
+    <t>478-10349-1-ND</t>
+  </si>
+  <si>
+    <t>478-8237-1-ND</t>
+  </si>
+  <si>
+    <t>478-11461-1-ND</t>
+  </si>
+  <si>
+    <t>399-8980-1-ND</t>
+  </si>
+  <si>
+    <t>SS2P6-M3/84AGICT-ND</t>
+  </si>
+  <si>
+    <t>490-10585-1-ND</t>
+  </si>
+  <si>
+    <t>1276AS-H-4R7M=P2</t>
+  </si>
+  <si>
+    <t>587-1623-1-ND</t>
+  </si>
+  <si>
+    <t>Taiyo Yuden</t>
+  </si>
+  <si>
+    <t>CBC3225T2R2MR</t>
+  </si>
+  <si>
+    <t>311-33GRCT-ND</t>
+  </si>
+  <si>
+    <t>311-10KGRCT-ND</t>
+  </si>
+  <si>
+    <t>311-10MGRCT-ND</t>
+  </si>
+  <si>
+    <t>311-499HRCT-ND</t>
+  </si>
+  <si>
+    <t>311-120KGRCT-ND</t>
+  </si>
+  <si>
+    <t>311-100KHRCT-ND</t>
+  </si>
+  <si>
+    <t>YAG3375CT-ND</t>
+  </si>
+  <si>
+    <t>1829-1005-ND</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -553,13 +625,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -574,16 +660,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -898,22 +993,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T39"/>
+  <dimension ref="A1:U39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="R15" sqref="R15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="44.25" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="31.42578125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="31.42578125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" customWidth="1"/>
+    <col min="6" max="9" width="0" hidden="1" customWidth="1"/>
+    <col min="13" max="17" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="1" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -971,1085 +1069,1214 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="2" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="N2">
+      <c r="N2" s="6">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="3" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
         <v>7</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H3">
+      <c r="E3" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="H3" s="4">
         <v>7.3999999999999996E-2</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="S3" t="s">
+      <c r="R3" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="S3" s="4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="4" spans="1:20" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="T3" s="4" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
         <v>6</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="4">
         <v>7.3999999999999996E-2</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="S4" t="s">
+      <c r="R4" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="S4" s="4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="5" spans="1:20" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="T4" s="4" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
         <v>7</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="4">
         <v>7.3999999999999996E-2</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J5" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="S5" t="s">
+      <c r="R5" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="S5" s="4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="6" spans="1:20" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="T5" s="4" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
         <v>2</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="4">
         <v>7.3999999999999996E-2</v>
       </c>
-      <c r="J6" t="s">
+      <c r="J6" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="S6" t="s">
+      <c r="R6" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="S6" s="4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="7" spans="1:20" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="T6" s="4" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
         <v>4</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="4">
         <v>7.3999999999999996E-2</v>
       </c>
-      <c r="J7" t="s">
+      <c r="J7" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="S7" t="s">
+      <c r="R7" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="S7" s="4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="8" spans="1:20" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="T7" s="4" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
         <v>4</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="4">
         <v>7.3999999999999996E-2</v>
       </c>
-      <c r="J8" t="s">
+      <c r="J8" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="S8" t="s">
+      <c r="R8" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="S8" s="4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="9" spans="1:20" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="T8" s="4" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
         <v>4</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="4">
         <v>7.3999999999999996E-2</v>
       </c>
-      <c r="J9" t="s">
+      <c r="J9" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="S9" t="s">
+      <c r="R9" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="S9" s="4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="10" spans="1:20" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10">
+      <c r="T9" s="4" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
         <v>4</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="4">
         <v>7.3999999999999996E-2</v>
       </c>
-      <c r="J10" t="s">
+      <c r="J10" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="S10" t="s">
+      <c r="R10" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="S10" s="4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="11" spans="1:20" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11">
+      <c r="T10" s="4" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
         <v>6</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="4">
         <v>0.8</v>
       </c>
-      <c r="J11" t="s">
+      <c r="J11" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="K11" t="s">
+      <c r="K11" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="L11" t="s">
+      <c r="L11" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="R11" t="s">
-        <v>46</v>
-      </c>
-      <c r="S11" t="s">
+      <c r="R11" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="S11" s="4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="12" spans="1:20" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12">
+      <c r="T11" s="4" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
         <v>2</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="4">
         <v>0.8</v>
       </c>
-      <c r="J12" t="s">
+      <c r="J12" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="K12" t="s">
+      <c r="K12" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="L12" t="s">
+      <c r="L12" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="R12" t="s">
-        <v>46</v>
-      </c>
-      <c r="S12" t="s">
+      <c r="R12" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="S12" s="4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="13" spans="1:20" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13">
+      <c r="T12" s="4" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
         <v>2</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="4">
         <v>7.3999999999999996E-2</v>
       </c>
-      <c r="J13" t="s">
+      <c r="J13" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="S13" t="s">
+      <c r="R13" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="S13" s="4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="14" spans="1:20" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14">
+      <c r="T13" s="4" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
         <v>4</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="K14" t="s">
+      <c r="K14" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="L14" t="s">
+      <c r="L14" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="N14">
+      <c r="N14" s="4">
         <v>0.68</v>
       </c>
-      <c r="R14" t="s">
-        <v>46</v>
-      </c>
-      <c r="T14" t="s">
+      <c r="R14" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="T14" s="4" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15">
+    <row r="15" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
         <v>3</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="H15">
+      <c r="H15" s="4">
         <v>0.39</v>
       </c>
-      <c r="K15" t="s">
+      <c r="K15" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="L15" t="s">
+      <c r="L15" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="R15" t="s">
-        <v>46</v>
-      </c>
-      <c r="T15" t="s">
+      <c r="R15" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="T15" s="8" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="16" spans="1:20" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16">
+      <c r="U15" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
         <v>1</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="K16" t="s">
+      <c r="K16" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="L16" t="s">
+      <c r="L16" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="N16">
+      <c r="N16" s="4">
         <v>1.66</v>
       </c>
-      <c r="R16" t="s">
-        <v>46</v>
-      </c>
-      <c r="T16" t="s">
+      <c r="R16" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="T16" s="4" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17">
+    <row r="17" spans="1:20" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
         <v>4</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="K17" t="s">
+      <c r="K17" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="L17" t="s">
+      <c r="L17" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="N17">
+      <c r="N17" s="4">
         <v>1.94</v>
       </c>
-      <c r="R17" t="s">
-        <v>46</v>
-      </c>
-      <c r="T17" t="s">
+      <c r="R17" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="T17" s="4" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18">
+    <row r="18" spans="1:20" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
         <v>1</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="G18" t="s">
+      <c r="G18" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="K18" t="s">
+      <c r="K18" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="L18" t="s">
+      <c r="L18" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="N18">
+      <c r="N18" s="4">
         <v>0.88</v>
       </c>
-      <c r="R18" t="s">
-        <v>46</v>
-      </c>
-      <c r="T18" t="s">
+      <c r="R18" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="T18" s="4" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="19" spans="1:20" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19">
+    <row r="19" spans="1:20" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="4">
         <v>1</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="G19" t="s">
+      <c r="G19" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="K19" t="s">
+      <c r="K19" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="L19" t="s">
+      <c r="L19" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="N19">
+      <c r="N19" s="4">
         <v>0.88</v>
       </c>
-      <c r="R19" t="s">
-        <v>46</v>
-      </c>
-      <c r="T19" t="s">
+      <c r="R19" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="T19" s="4" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="20" spans="1:20" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20">
+    <row r="20" spans="1:20" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="4">
         <v>1</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="G20" t="s">
+      <c r="G20" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="K20" t="s">
+      <c r="K20" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="L20" t="s">
+      <c r="L20" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="N20">
+      <c r="N20" s="4">
         <v>0.88</v>
       </c>
-      <c r="R20" t="s">
-        <v>46</v>
-      </c>
-      <c r="T20" t="s">
+      <c r="R20" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="T20" s="4" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="21" spans="1:20" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21">
+    <row r="21" spans="1:20" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="4">
         <v>3</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="K21" t="s">
+      <c r="K21" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="L21" t="s">
+      <c r="L21" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="N21">
+      <c r="N21" s="4">
         <v>1.24</v>
       </c>
-      <c r="R21" t="s">
-        <v>46</v>
-      </c>
-      <c r="T21" t="s">
+      <c r="R21" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="T21" s="4" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="22" spans="1:20" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22">
+    <row r="22" spans="1:20" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="4">
         <v>1</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="O22">
+      <c r="L22" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="O22" s="4">
         <v>1206</v>
       </c>
-    </row>
-    <row r="23" spans="1:20" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23">
+      <c r="R22" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="T22" s="4" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="4">
         <v>1</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="O23">
+      <c r="K23" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="L23" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="O23" s="4">
         <v>1206</v>
       </c>
-    </row>
-    <row r="24" spans="1:20" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24">
+      <c r="R23" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="T23" s="4" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="4">
         <v>12</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="4">
         <v>33</v>
       </c>
-      <c r="M24">
+      <c r="M24" s="4">
         <v>603</v>
       </c>
-      <c r="N24">
+      <c r="N24" s="4">
         <v>5.8999999999999997E-2</v>
       </c>
-      <c r="P24" s="2">
+      <c r="P24" s="9">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="25" spans="1:20" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25">
+      <c r="R24" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="T24" s="4" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="4">
         <v>11</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B25" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E25" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="M25">
+      <c r="M25" s="4">
         <v>603</v>
       </c>
-      <c r="N25">
+      <c r="N25" s="4">
         <v>5.8999999999999997E-2</v>
       </c>
-      <c r="P25" s="2">
+      <c r="P25" s="9">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="26" spans="1:20" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26">
+      <c r="R25" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="T25" s="4" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="4">
         <v>1</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E26" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="M26">
+      <c r="M26" s="4">
         <v>603</v>
       </c>
-      <c r="N26">
+      <c r="N26" s="4">
         <v>5.8999999999999997E-2</v>
       </c>
-      <c r="P26" s="2">
+      <c r="P26" s="9">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="27" spans="1:20" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27">
+      <c r="R26" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="T26" s="4" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="4">
         <v>16</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E27">
+      <c r="E27" s="4">
         <v>500</v>
       </c>
-      <c r="N27">
+      <c r="N27" s="4">
         <v>5.8999999999999997E-2</v>
       </c>
-    </row>
-    <row r="28" spans="1:20" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28">
+      <c r="R27" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="T27" s="4" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="4">
         <v>1</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B28" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D28" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E28" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="M28">
+      <c r="M28" s="4">
         <v>1206</v>
       </c>
-      <c r="N28">
+      <c r="N28" s="4">
         <v>0.03</v>
       </c>
-      <c r="P28" s="2">
+      <c r="P28" s="9">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="29" spans="1:20" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29">
+      <c r="R28" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="T28" s="4" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="4">
         <v>1</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B29" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D29" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E29" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="M29">
+      <c r="M29" s="4">
         <v>603</v>
       </c>
-      <c r="N29">
+      <c r="N29" s="4">
         <v>5.8999999999999997E-2</v>
       </c>
-      <c r="P29" s="2">
+      <c r="P29" s="9">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="30" spans="1:20" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30">
+      <c r="R29" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="4">
         <v>1</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B30" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D30" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E30" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="M30">
+      <c r="M30" s="4">
         <v>603</v>
       </c>
-      <c r="N30">
+      <c r="N30" s="4">
         <v>5.8999999999999997E-2</v>
       </c>
-      <c r="P30" s="2">
+      <c r="P30" s="9">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="31" spans="1:20" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31">
+      <c r="R30" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="T30" s="4" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="4">
         <v>2</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B31" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D31" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E31" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="M31">
+      <c r="M31" s="4">
         <v>603</v>
       </c>
-      <c r="N31">
+      <c r="N31" s="4">
         <v>5.8999999999999997E-2</v>
       </c>
-      <c r="P31" s="2">
+      <c r="P31" s="9">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="32" spans="1:20" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32">
+      <c r="R31" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="T31" s="4" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="4">
         <v>2</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B32" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D32" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E32" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="K32" t="s">
+      <c r="K32" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="L32" t="s">
+      <c r="L32" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="R32" t="s">
-        <v>46</v>
-      </c>
-      <c r="T32" t="s">
+      <c r="R32" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="4">
+        <v>1</v>
+      </c>
+      <c r="B33" s="5" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="33" spans="1:20" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33">
+      <c r="C33" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="K33" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="L33" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="N33" s="4">
+        <v>5.45</v>
+      </c>
+      <c r="R33" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="T33" s="4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="4">
         <v>1</v>
       </c>
-      <c r="B33" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="C33" t="s">
-        <v>127</v>
-      </c>
-      <c r="D33" t="s">
-        <v>128</v>
-      </c>
-      <c r="E33" t="s">
-        <v>127</v>
-      </c>
-      <c r="K33" t="s">
-        <v>129</v>
-      </c>
-      <c r="L33" t="s">
-        <v>130</v>
-      </c>
-      <c r="N33">
-        <v>5.45</v>
-      </c>
-      <c r="R33" t="s">
-        <v>46</v>
-      </c>
-      <c r="T33" t="s">
+      <c r="B34" s="5" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="34" spans="1:20" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34">
+      <c r="C34" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="K34" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="L34" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="N34" s="4">
+        <v>6.25</v>
+      </c>
+      <c r="R34" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="T34" s="4" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="4">
         <v>1</v>
       </c>
-      <c r="B34" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="C34" t="s">
-        <v>133</v>
-      </c>
-      <c r="D34" t="s">
-        <v>134</v>
-      </c>
-      <c r="E34" t="s">
-        <v>133</v>
-      </c>
-      <c r="K34" t="s">
-        <v>135</v>
-      </c>
-      <c r="L34" t="s">
-        <v>136</v>
-      </c>
-      <c r="N34">
-        <v>6.25</v>
-      </c>
-      <c r="R34" t="s">
-        <v>46</v>
-      </c>
-      <c r="T34" t="s">
+      <c r="B35" s="5" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="35" spans="1:20" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35">
+      <c r="C35" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="K35" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="L35" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="N35" s="4">
+        <v>1.83</v>
+      </c>
+      <c r="R35" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="T35" s="4" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="4">
         <v>1</v>
       </c>
-      <c r="B35" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="C35" t="s">
-        <v>139</v>
-      </c>
-      <c r="D35" t="s">
-        <v>140</v>
-      </c>
-      <c r="E35" t="s">
-        <v>139</v>
-      </c>
-      <c r="K35" t="s">
-        <v>141</v>
-      </c>
-      <c r="L35" t="s">
-        <v>142</v>
-      </c>
-      <c r="N35">
-        <v>1.83</v>
-      </c>
-      <c r="R35" t="s">
-        <v>46</v>
-      </c>
-      <c r="T35" t="s">
+      <c r="B36" s="5" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="36" spans="1:20" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36">
+      <c r="C36" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="K36" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="L36" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="N36" s="4">
+        <v>45.88</v>
+      </c>
+      <c r="R36" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="T36" s="4" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="4">
         <v>1</v>
       </c>
-      <c r="B36" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="C36" t="s">
-        <v>145</v>
-      </c>
-      <c r="D36" t="s">
-        <v>146</v>
-      </c>
-      <c r="E36" t="s">
-        <v>145</v>
-      </c>
-      <c r="K36" t="s">
-        <v>147</v>
-      </c>
-      <c r="L36" t="s">
+      <c r="B37" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="N36">
-        <v>45.88</v>
-      </c>
-      <c r="R36" t="s">
-        <v>46</v>
-      </c>
-      <c r="T36" t="s">
+      <c r="C37" s="4" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="37" spans="1:20" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37">
+      <c r="D37" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="K37" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="L37" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="N37" s="4">
+        <v>0.73</v>
+      </c>
+      <c r="R37" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="T37" s="4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="4">
         <v>1</v>
       </c>
-      <c r="B37" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="C37" t="s">
-        <v>151</v>
-      </c>
-      <c r="D37" t="s">
-        <v>152</v>
-      </c>
-      <c r="E37" t="s">
-        <v>151</v>
-      </c>
-      <c r="K37" t="s">
-        <v>153</v>
-      </c>
-      <c r="L37" t="s">
+      <c r="B38" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="N37">
-        <v>0.73</v>
-      </c>
-      <c r="R37" t="s">
-        <v>46</v>
-      </c>
-      <c r="T37" t="s">
+      <c r="C38" s="4" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="38" spans="1:20" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38">
+      <c r="D38" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="K38" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="L38" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="N38" s="4">
+        <v>4.79</v>
+      </c>
+      <c r="R38" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="T38" s="4" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="4">
         <v>1</v>
       </c>
-      <c r="B38" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="C38" t="s">
-        <v>157</v>
-      </c>
-      <c r="D38" t="s">
-        <v>158</v>
-      </c>
-      <c r="E38" t="s">
-        <v>157</v>
-      </c>
-      <c r="K38" t="s">
-        <v>159</v>
-      </c>
-      <c r="L38" t="s">
+      <c r="B39" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="N38">
-        <v>4.79</v>
-      </c>
-      <c r="R38" t="s">
-        <v>46</v>
-      </c>
-      <c r="T38" t="s">
+      <c r="C39" s="4" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="39" spans="1:20" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>1</v>
-      </c>
-      <c r="B39" s="4" t="s">
+      <c r="D39" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="C39" t="s">
+      <c r="E39" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="K39" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="D39" t="s">
+      <c r="L39" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="E39" t="s">
-        <v>163</v>
-      </c>
-      <c r="K39" t="s">
+      <c r="N39" s="4">
+        <v>0.76</v>
+      </c>
+      <c r="Q39" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="L39" t="s">
+      <c r="R39" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="T39" s="4" t="s">
         <v>166</v>
-      </c>
-      <c r="N39">
-        <v>0.76</v>
-      </c>
-      <c r="Q39" t="s">
-        <v>167</v>
-      </c>
-      <c r="R39" t="s">
-        <v>46</v>
-      </c>
-      <c r="T39" t="s">
-        <v>168</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removed errorneous polygon from dsp_pid.brd that shorted VIN to GND. Updated bom.xlsx
</commit_message>
<xml_diff>
--- a/bom.xlsx
+++ b/bom.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="24000" windowHeight="10380"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="10380"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="219">
   <si>
     <t>QTY</t>
   </si>
@@ -603,13 +603,91 @@
   </si>
   <si>
     <t>1829-1005-ND</t>
+  </si>
+  <si>
+    <t>SOLIDMODEL</t>
+  </si>
+  <si>
+    <t>SOLIDWORKS_CONFIG</t>
+  </si>
+  <si>
+    <t>SOLIDWORKS_FILE</t>
+  </si>
+  <si>
+    <t>C1,C2,C35,C36,</t>
+  </si>
+  <si>
+    <t>0.1U</t>
+  </si>
+  <si>
+    <t>CAP_NP_0603.g</t>
+  </si>
+  <si>
+    <t>SIZE_0603</t>
+  </si>
+  <si>
+    <t>ChipCapacitor.SLDASM</t>
+  </si>
+  <si>
+    <t>C4,C5,C6,C7,C8,C9,C11,C14,C15,C34,C49,</t>
+  </si>
+  <si>
+    <t>CAP_TANT_SIZE_A.g</t>
+  </si>
+  <si>
+    <t>SIZE_A</t>
+  </si>
+  <si>
+    <t>TantalumCap.SLDASM</t>
+  </si>
+  <si>
+    <t>R1,R4,R5,R6,R7,R8,R10,R15,R16,R17,R19,R36,R46,</t>
+  </si>
+  <si>
+    <t>res0603.g</t>
+  </si>
+  <si>
+    <t>ChipResistor.SLDASM</t>
+  </si>
+  <si>
+    <t>R2,R3,R9,R11,R12,R13,R14,R38,R43,R44,R45,R47,</t>
+  </si>
+  <si>
+    <t>res1206.g</t>
+  </si>
+  <si>
+    <t>SIZE_01206</t>
+  </si>
+  <si>
+    <t>OPA1679IPWR-ND</t>
+  </si>
+  <si>
+    <t>LFCSP.SLDASM</t>
+  </si>
+  <si>
+    <t>1829-1000-ND</t>
+  </si>
+  <si>
+    <t>U9,</t>
+  </si>
+  <si>
+    <t>SOT23-3</t>
+  </si>
+  <si>
+    <t>SUPRVISOR-APX803S</t>
+  </si>
+  <si>
+    <t>APX803S-31SA-7</t>
+  </si>
+  <si>
+    <t>APX803S-31SA-7DICT-ND</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -626,6 +704,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <strike/>
       <sz val="11"/>
       <color theme="1"/>
@@ -660,25 +747,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -993,1291 +1081,2692 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U39"/>
+  <dimension ref="A1:AR41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R15" sqref="R15"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="R43" sqref="R43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="31.42578125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" customWidth="1"/>
-    <col min="6" max="9" width="0" hidden="1" customWidth="1"/>
-    <col min="13" max="17" width="0" hidden="1" customWidth="1"/>
+    <col min="20" max="22" width="0" hidden="1" customWidth="1"/>
+    <col min="24" max="24" width="0" hidden="1" customWidth="1"/>
+    <col min="25" max="25" width="31.42578125" style="2" hidden="1" customWidth="1"/>
+    <col min="26" max="26" width="0" hidden="1" customWidth="1"/>
+    <col min="27" max="27" width="15.28515625" hidden="1" customWidth="1"/>
+    <col min="28" max="40" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:44" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1">
+        <v>15</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="X1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="AA1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="AB1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1">
+      <c r="AC1" s="9">
         <v>15</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="AD1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="AE1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="AF1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="AG1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="AH1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="AI1" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6">
-        <v>1</v>
-      </c>
-      <c r="B2" s="7" t="s">
+    <row r="2" spans="1:44" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="H2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="M2" s="4">
+        <v>10</v>
+      </c>
+      <c r="X2" s="4">
+        <v>1</v>
+      </c>
+      <c r="Y2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="Z2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="AF2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="N2" s="6">
+      <c r="AK2" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
+    <row r="3" spans="1:44" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="G3" s="3">
+        <v>7.3999999999999996E-2</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="U3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="X3" s="6">
         <v>7</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="Y3" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="Z3" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="AA3" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="AB3" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="H3" s="4">
+      <c r="AC3" s="6"/>
+      <c r="AD3" s="6"/>
+      <c r="AE3" s="6">
         <v>7.3999999999999996E-2</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="AF3" s="6"/>
+      <c r="AG3" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="R3" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="S3" s="4" t="s">
+      <c r="AH3" s="6"/>
+      <c r="AI3" s="6"/>
+      <c r="AO3" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="AP3" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="T3" s="4" t="s">
+      <c r="AQ3" s="3" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="4" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
+    <row r="4" spans="1:44" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4">
         <v>6</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" s="3">
+        <v>7.3999999999999996E-2</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="U4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="X4" s="6">
+        <v>6</v>
+      </c>
+      <c r="Y4" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z4" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="AA4" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="AB4" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="H4" s="4">
+      <c r="AC4" s="6"/>
+      <c r="AD4" s="6"/>
+      <c r="AE4" s="6">
         <v>7.3999999999999996E-2</v>
       </c>
-      <c r="J4" s="4" t="s">
+      <c r="AF4" s="6"/>
+      <c r="AG4" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="R4" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="S4" s="4" t="s">
+      <c r="AH4" s="6"/>
+      <c r="AI4" s="6"/>
+      <c r="AO4" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="AP4" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="T4" s="4" t="s">
+      <c r="AQ4" s="3" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="5" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
+    <row r="5" spans="1:44" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>11</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" s="3">
+        <v>7.3999999999999996E-2</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="O5" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="P5" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q5" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="U5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="X5" s="6">
         <v>7</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="Y5" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="Z5" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="AA5" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="AB5" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="H5" s="4">
+      <c r="AC5" s="6"/>
+      <c r="AD5" s="6"/>
+      <c r="AE5" s="6">
         <v>7.3999999999999996E-2</v>
       </c>
-      <c r="J5" s="4" t="s">
+      <c r="AF5" s="6"/>
+      <c r="AG5" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="R5" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="S5" s="4" t="s">
+      <c r="AH5" s="6"/>
+      <c r="AI5" s="6"/>
+      <c r="AO5" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="AP5" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="T5" s="4" t="s">
+      <c r="AQ5" s="3" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="6" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
+    <row r="6" spans="1:44" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6">
         <v>2</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" s="3">
+        <v>7.3999999999999996E-2</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="O6" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="P6" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q6" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="U6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="X6" s="6">
+        <v>2</v>
+      </c>
+      <c r="Y6" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z6" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="AA6" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="AB6" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="H6" s="4">
+      <c r="AC6" s="6"/>
+      <c r="AD6" s="6"/>
+      <c r="AE6" s="6">
         <v>7.3999999999999996E-2</v>
       </c>
-      <c r="J6" s="4" t="s">
+      <c r="AF6" s="6"/>
+      <c r="AG6" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="R6" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="S6" s="4" t="s">
+      <c r="AH6" s="6"/>
+      <c r="AI6" s="6"/>
+      <c r="AO6" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="AP6" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="T6" s="4" t="s">
+      <c r="AQ6" s="3" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="7" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
+    <row r="7" spans="1:44" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7">
         <v>4</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G7" s="3">
+        <v>7.3999999999999996E-2</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="O7" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="P7" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q7" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="U7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="X7" s="6">
+        <v>4</v>
+      </c>
+      <c r="Y7" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="Z7" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="AA7" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="AB7" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="H7" s="4">
+      <c r="AC7" s="6"/>
+      <c r="AD7" s="6"/>
+      <c r="AE7" s="6">
         <v>7.3999999999999996E-2</v>
       </c>
-      <c r="J7" s="4" t="s">
+      <c r="AF7" s="6"/>
+      <c r="AG7" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="R7" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="S7" s="4" t="s">
+      <c r="AH7" s="6"/>
+      <c r="AI7" s="6"/>
+      <c r="AO7" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="AP7" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="T7" s="4" t="s">
+      <c r="AQ7" s="3" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="8" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
+    <row r="8" spans="1:44" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8">
         <v>4</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G8" s="3">
+        <v>7.3999999999999996E-2</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="O8" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="P8" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q8" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="U8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="X8" s="6">
+        <v>4</v>
+      </c>
+      <c r="Y8" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z8" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="AA8" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="AB8" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="H8" s="4">
+      <c r="AC8" s="6"/>
+      <c r="AD8" s="6"/>
+      <c r="AE8" s="6">
         <v>7.3999999999999996E-2</v>
       </c>
-      <c r="J8" s="4" t="s">
+      <c r="AF8" s="6"/>
+      <c r="AG8" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="R8" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="S8" s="4" t="s">
+      <c r="AH8" s="6"/>
+      <c r="AI8" s="6"/>
+      <c r="AO8" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="AP8" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="T8" s="4" t="s">
+      <c r="AQ8" s="3" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="9" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4">
+    <row r="9" spans="1:44" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9">
         <v>4</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G9" s="3">
+        <v>7.3999999999999996E-2</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="O9" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="P9" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q9" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="U9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="X9" s="6">
+        <v>4</v>
+      </c>
+      <c r="Y9" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z9" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="AA9" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="AB9" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="H9" s="4">
+      <c r="AC9" s="6"/>
+      <c r="AD9" s="6"/>
+      <c r="AE9" s="6">
         <v>7.3999999999999996E-2</v>
       </c>
-      <c r="J9" s="4" t="s">
+      <c r="AF9" s="6"/>
+      <c r="AG9" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="R9" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="S9" s="4" t="s">
+      <c r="AH9" s="6"/>
+      <c r="AI9" s="6"/>
+      <c r="AO9" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="AP9" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="T9" s="4" t="s">
+      <c r="AQ9" s="3" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="10" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="4">
+    <row r="10" spans="1:44" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10">
         <v>4</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G10" s="3">
+        <v>7.3999999999999996E-2</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="O10" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="P10" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q10" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="U10" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="X10" s="6">
+        <v>4</v>
+      </c>
+      <c r="Y10" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z10" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="AA10" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="AB10" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="H10" s="4">
+      <c r="AC10" s="6"/>
+      <c r="AD10" s="6"/>
+      <c r="AE10" s="6">
         <v>7.3999999999999996E-2</v>
       </c>
-      <c r="J10" s="4" t="s">
+      <c r="AF10" s="6"/>
+      <c r="AG10" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="R10" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="S10" s="4" t="s">
+      <c r="AH10" s="6"/>
+      <c r="AI10" s="6"/>
+      <c r="AO10" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="AP10" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="T10" s="4" t="s">
+      <c r="AQ10" s="3" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="11" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="4">
+    <row r="11" spans="1:44" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11">
         <v>6</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G11" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="O11" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="P11" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="Q11" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="T11" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="U11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="X11" s="6">
+        <v>6</v>
+      </c>
+      <c r="Y11" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z11" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="AA11" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="AB11" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="H11" s="4">
+      <c r="AC11" s="6"/>
+      <c r="AD11" s="6"/>
+      <c r="AE11" s="6">
         <v>0.8</v>
       </c>
-      <c r="J11" s="4" t="s">
+      <c r="AF11" s="6"/>
+      <c r="AG11" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="K11" s="4" t="s">
+      <c r="AH11" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="L11" s="4" t="s">
+      <c r="AI11" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="R11" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="S11" s="4" t="s">
+      <c r="AO11" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="AP11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="T11" s="4" t="s">
+      <c r="AQ11" s="3" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="12" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="4">
+    <row r="12" spans="1:44" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12">
         <v>2</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="G12" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="O12" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="P12" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="Q12" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="T12" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="U12" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="X12" s="6">
+        <v>2</v>
+      </c>
+      <c r="Y12" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="Z12" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="AA12" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="AB12" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="H12" s="4">
+      <c r="AC12" s="6"/>
+      <c r="AD12" s="6"/>
+      <c r="AE12" s="6">
         <v>0.8</v>
       </c>
-      <c r="J12" s="4" t="s">
+      <c r="AF12" s="6"/>
+      <c r="AG12" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="K12" s="4" t="s">
+      <c r="AH12" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="L12" s="4" t="s">
+      <c r="AI12" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="R12" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="S12" s="4" t="s">
+      <c r="AO12" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="AP12" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="T12" s="4" t="s">
+      <c r="AQ12" s="3" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="13" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="4">
+    <row r="13" spans="1:44" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13">
         <v>2</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G13" s="3">
+        <v>7.3999999999999996E-2</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="O13" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="P13" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q13" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="U13" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="X13" s="6">
+        <v>2</v>
+      </c>
+      <c r="Y13" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z13" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="AA13" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="AB13" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="H13" s="4">
+      <c r="AC13" s="6"/>
+      <c r="AD13" s="6"/>
+      <c r="AE13" s="6">
         <v>7.3999999999999996E-2</v>
       </c>
-      <c r="J13" s="4" t="s">
+      <c r="AF13" s="6"/>
+      <c r="AG13" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="R13" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="S13" s="4" t="s">
+      <c r="AH13" s="6"/>
+      <c r="AI13" s="6"/>
+      <c r="AO13" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="AP13" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="T13" s="4" t="s">
+      <c r="AQ13" s="3" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="14" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="4">
+    <row r="14" spans="1:44" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14">
         <v>4</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D14" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="J14" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="K14" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="M14" s="3">
+        <v>0.68</v>
+      </c>
+      <c r="T14" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="V14" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="X14" s="6">
+        <v>4</v>
+      </c>
+      <c r="Y14" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z14" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA14" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="AB14" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="K14" s="4" t="s">
+      <c r="AC14" s="6"/>
+      <c r="AD14" s="6"/>
+      <c r="AE14" s="6"/>
+      <c r="AF14" s="6"/>
+      <c r="AG14" s="6"/>
+      <c r="AH14" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="L14" s="4" t="s">
+      <c r="AI14" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="N14" s="4">
+      <c r="AK14" s="3">
         <v>0.68</v>
       </c>
-      <c r="R14" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="T14" s="4" t="s">
+      <c r="AO14" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="AQ14" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="4">
+    <row r="15" spans="1:44" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15">
         <v>3</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D15" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="G15" s="3">
+        <v>0.39</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="K15" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="T15" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="V15" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="X15" s="6">
+        <v>3</v>
+      </c>
+      <c r="Y15" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="Z15" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA15" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="AB15" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="H15" s="4">
+      <c r="AC15" s="6"/>
+      <c r="AD15" s="6"/>
+      <c r="AE15" s="6">
         <v>0.39</v>
       </c>
-      <c r="K15" s="4" t="s">
+      <c r="AF15" s="6"/>
+      <c r="AG15" s="6"/>
+      <c r="AH15" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="L15" s="4" t="s">
+      <c r="AI15" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="R15" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="T15" s="8" t="s">
+      <c r="AO15" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="AQ15" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="U15" s="4" t="s">
+      <c r="AR15" s="3" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="16" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="4">
-        <v>1</v>
-      </c>
-      <c r="B16" s="5" t="s">
+    <row r="16" spans="1:44" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D16" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="J16" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="K16" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="M16" s="3">
+        <v>1.66</v>
+      </c>
+      <c r="T16" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="V16" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="X16" s="6">
+        <v>1</v>
+      </c>
+      <c r="Y16" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z16" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AA16" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="AB16" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="K16" s="4" t="s">
+      <c r="AC16" s="6"/>
+      <c r="AD16" s="6"/>
+      <c r="AE16" s="6"/>
+      <c r="AF16" s="6"/>
+      <c r="AG16" s="6"/>
+      <c r="AH16" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="L16" s="4" t="s">
+      <c r="AI16" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="N16" s="4">
+      <c r="AK16" s="3">
         <v>1.66</v>
       </c>
-      <c r="R16" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="T16" s="4" t="s">
+      <c r="AO16" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="AQ16" s="3" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="17" spans="1:20" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="4">
+    <row r="17" spans="1:43" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17">
         <v>4</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D17" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="J17" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="K17" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="M17" s="3">
+        <v>1.94</v>
+      </c>
+      <c r="T17" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="V17" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="X17" s="6">
+        <v>4</v>
+      </c>
+      <c r="Y17" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="Z17" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="AA17" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="AB17" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="K17" s="4" t="s">
+      <c r="AC17" s="6"/>
+      <c r="AD17" s="6"/>
+      <c r="AE17" s="6"/>
+      <c r="AF17" s="6"/>
+      <c r="AG17" s="6"/>
+      <c r="AH17" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="L17" s="4" t="s">
+      <c r="AI17" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="N17" s="4">
+      <c r="AK17" s="3">
         <v>1.94</v>
       </c>
-      <c r="R17" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="T17" s="4" t="s">
+      <c r="AO17" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="AQ17" s="3" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="18" spans="1:20" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="4">
-        <v>1</v>
-      </c>
-      <c r="B18" s="5" t="s">
+    <row r="18" spans="1:43" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D18" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="F18" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="K18" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="M18" s="3">
+        <v>0.88</v>
+      </c>
+      <c r="T18" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="V18" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="X18" s="6">
+        <v>1</v>
+      </c>
+      <c r="Y18" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z18" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="AA18" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="E18" s="4" t="s">
+      <c r="AB18" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="G18" s="4" t="s">
+      <c r="AC18" s="6"/>
+      <c r="AD18" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="K18" s="4" t="s">
+      <c r="AE18" s="6"/>
+      <c r="AF18" s="6"/>
+      <c r="AG18" s="6"/>
+      <c r="AH18" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="L18" s="4" t="s">
+      <c r="AI18" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="N18" s="4">
+      <c r="AK18" s="3">
         <v>0.88</v>
       </c>
-      <c r="R18" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="T18" s="4" t="s">
+      <c r="AO18" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="AQ18" s="3" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="19" spans="1:20" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="4">
-        <v>1</v>
-      </c>
-      <c r="B19" s="5" t="s">
+    <row r="19" spans="1:43" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>1</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D19" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="F19" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="K19" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="M19" s="3">
+        <v>0.88</v>
+      </c>
+      <c r="T19" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="V19" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="X19" s="6">
+        <v>1</v>
+      </c>
+      <c r="Y19" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="Z19" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="AA19" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="AB19" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="G19" s="4" t="s">
+      <c r="AC19" s="6"/>
+      <c r="AD19" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="K19" s="4" t="s">
+      <c r="AE19" s="6"/>
+      <c r="AF19" s="6"/>
+      <c r="AG19" s="6"/>
+      <c r="AH19" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="L19" s="4" t="s">
+      <c r="AI19" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="N19" s="4">
+      <c r="AK19" s="3">
         <v>0.88</v>
       </c>
-      <c r="R19" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="T19" s="4" t="s">
+      <c r="AO19" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="AQ19" s="3" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="20" spans="1:20" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="4">
-        <v>1</v>
-      </c>
-      <c r="B20" s="5" t="s">
+    <row r="20" spans="1:43" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>1</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D20" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="F20" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="K20" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="M20" s="3">
+        <v>0.88</v>
+      </c>
+      <c r="T20" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="V20" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="X20" s="6">
+        <v>1</v>
+      </c>
+      <c r="Y20" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z20" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="AA20" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="E20" s="4" t="s">
+      <c r="AB20" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="G20" s="4" t="s">
+      <c r="AC20" s="6"/>
+      <c r="AD20" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="K20" s="4" t="s">
+      <c r="AE20" s="6"/>
+      <c r="AF20" s="6"/>
+      <c r="AG20" s="6"/>
+      <c r="AH20" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="L20" s="4" t="s">
+      <c r="AI20" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="N20" s="4">
+      <c r="AK20" s="3">
         <v>0.88</v>
       </c>
-      <c r="R20" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="T20" s="4" t="s">
+      <c r="AO20" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="AQ20" s="3" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="21" spans="1:20" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="4">
+    <row r="21" spans="1:43" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21">
         <v>3</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C21" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D21" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="J21" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="K21" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="M21" s="3">
+        <v>1.24</v>
+      </c>
+      <c r="T21" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="V21" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="X21" s="6">
+        <v>3</v>
+      </c>
+      <c r="Y21" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="Z21" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="AA21" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="AB21" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="K21" s="4" t="s">
+      <c r="AC21" s="6"/>
+      <c r="AD21" s="6"/>
+      <c r="AE21" s="6"/>
+      <c r="AF21" s="6"/>
+      <c r="AG21" s="6"/>
+      <c r="AH21" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="L21" s="4" t="s">
+      <c r="AI21" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="N21" s="4">
+      <c r="AK21" s="3">
         <v>1.24</v>
       </c>
-      <c r="R21" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="T21" s="4" t="s">
+      <c r="AO21" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="AQ21" s="3" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="22" spans="1:20" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="4">
-        <v>1</v>
-      </c>
-      <c r="B22" s="5" t="s">
+    <row r="22" spans="1:43" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>1</v>
+      </c>
+      <c r="B22" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C22" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="N22" s="3">
+        <v>1206</v>
+      </c>
+      <c r="X22" s="6">
+        <v>1</v>
+      </c>
+      <c r="Y22" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="Z22" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="AA22" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="E22" s="4" t="s">
+      <c r="AB22" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="L22" s="4" t="s">
+      <c r="AC22" s="6"/>
+      <c r="AD22" s="6"/>
+      <c r="AE22" s="6"/>
+      <c r="AF22" s="6"/>
+      <c r="AG22" s="6"/>
+      <c r="AH22" s="6"/>
+      <c r="AI22" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="O22" s="4">
+      <c r="AL22" s="3">
         <v>1206</v>
       </c>
-      <c r="R22" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="T22" s="4" t="s">
+      <c r="AO22" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="AQ22" s="3" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="23" spans="1:20" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="4">
-        <v>1</v>
-      </c>
-      <c r="B23" s="5" t="s">
+    <row r="23" spans="1:43" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>1</v>
+      </c>
+      <c r="B23" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C23" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="N23" s="3">
+        <v>1206</v>
+      </c>
+      <c r="X23" s="6">
+        <v>1</v>
+      </c>
+      <c r="Y23" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="Z23" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="AA23" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="E23" s="4" t="s">
+      <c r="AB23" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="K23" s="4" t="s">
+      <c r="AC23" s="6"/>
+      <c r="AD23" s="6"/>
+      <c r="AE23" s="6"/>
+      <c r="AF23" s="6"/>
+      <c r="AG23" s="6"/>
+      <c r="AH23" s="6" t="s">
         <v>183</v>
       </c>
-      <c r="L23" s="4" t="s">
+      <c r="AI23" s="6" t="s">
         <v>184</v>
       </c>
-      <c r="O23" s="4">
+      <c r="AL23" s="3">
         <v>1206</v>
       </c>
-      <c r="R23" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="T23" s="4" t="s">
+      <c r="AO23" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="AQ23" s="3" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="24" spans="1:20" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="4">
+    <row r="24" spans="1:43" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>13</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D24" s="3">
+        <v>33</v>
+      </c>
+      <c r="L24" s="3">
+        <v>603</v>
+      </c>
+      <c r="M24" s="3">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="O24" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="P24" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q24" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="R24" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="X24" s="6">
         <v>12</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="Y24" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="Z24" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="D24" s="4" t="s">
+      <c r="AA24" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E24" s="4">
+      <c r="AB24" s="6">
         <v>33</v>
       </c>
-      <c r="M24" s="4">
+      <c r="AC24" s="6"/>
+      <c r="AD24" s="6"/>
+      <c r="AE24" s="6"/>
+      <c r="AF24" s="6"/>
+      <c r="AG24" s="6"/>
+      <c r="AH24" s="6"/>
+      <c r="AI24" s="6"/>
+      <c r="AJ24" s="3">
         <v>603</v>
       </c>
-      <c r="N24" s="4">
+      <c r="AK24" s="3">
         <v>5.8999999999999997E-2</v>
       </c>
-      <c r="P24" s="9">
+      <c r="AM24" s="7">
         <v>0.01</v>
       </c>
-      <c r="R24" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="T24" s="4" t="s">
+      <c r="AO24" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="AQ24" s="3" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="25" spans="1:20" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="4">
+    <row r="25" spans="1:43" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>12</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="L25" s="3">
+        <v>603</v>
+      </c>
+      <c r="M25" s="3">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="O25" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="P25" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q25" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="R25" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="X25" s="6">
         <v>11</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="Y25" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="Z25" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="D25" s="4" t="s">
+      <c r="AA25" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E25" s="4" t="s">
+      <c r="AB25" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="M25" s="4">
+      <c r="AC25" s="6"/>
+      <c r="AD25" s="6"/>
+      <c r="AE25" s="6"/>
+      <c r="AF25" s="6"/>
+      <c r="AG25" s="6"/>
+      <c r="AH25" s="6"/>
+      <c r="AI25" s="6"/>
+      <c r="AJ25" s="3">
         <v>603</v>
       </c>
-      <c r="N25" s="4">
+      <c r="AK25" s="3">
         <v>5.8999999999999997E-2</v>
       </c>
-      <c r="P25" s="9">
+      <c r="AM25" s="7">
         <v>0.01</v>
       </c>
-      <c r="R25" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="T25" s="4" t="s">
+      <c r="AO25" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="AQ25" s="3" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="26" spans="1:20" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="4">
-        <v>1</v>
-      </c>
-      <c r="B26" s="5" t="s">
+    <row r="26" spans="1:43" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>1</v>
+      </c>
+      <c r="B26" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="C26" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="L26" s="3">
+        <v>603</v>
+      </c>
+      <c r="M26" s="3">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="O26" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="P26" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q26" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="R26" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="X26" s="6">
+        <v>1</v>
+      </c>
+      <c r="Y26" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="Z26" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="D26" s="4" t="s">
+      <c r="AA26" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E26" s="4" t="s">
+      <c r="AB26" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="M26" s="4">
+      <c r="AC26" s="6"/>
+      <c r="AD26" s="6"/>
+      <c r="AE26" s="6"/>
+      <c r="AF26" s="6"/>
+      <c r="AG26" s="6"/>
+      <c r="AH26" s="6"/>
+      <c r="AI26" s="6"/>
+      <c r="AJ26" s="3">
         <v>603</v>
       </c>
-      <c r="N26" s="4">
+      <c r="AK26" s="3">
         <v>5.8999999999999997E-2</v>
       </c>
-      <c r="P26" s="9">
+      <c r="AM26" s="7">
         <v>0.01</v>
       </c>
-      <c r="R26" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="T26" s="4" t="s">
+      <c r="AO26" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="AQ26" s="3" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="27" spans="1:20" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="4">
+    <row r="27" spans="1:43" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A27">
         <v>16</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="B27" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="C27" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D27" s="3">
+        <v>500</v>
+      </c>
+      <c r="M27" s="3">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="O27" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="P27" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q27" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="X27" s="6">
+        <v>16</v>
+      </c>
+      <c r="Y27" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="Z27" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="D27" s="4" t="s">
+      <c r="AA27" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E27" s="4">
+      <c r="AB27" s="6">
         <v>500</v>
       </c>
-      <c r="N27" s="4">
+      <c r="AC27" s="6"/>
+      <c r="AD27" s="6"/>
+      <c r="AE27" s="6"/>
+      <c r="AF27" s="6"/>
+      <c r="AG27" s="6"/>
+      <c r="AH27" s="6"/>
+      <c r="AI27" s="6"/>
+      <c r="AK27" s="3">
         <v>5.8999999999999997E-2</v>
       </c>
-      <c r="R27" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="T27" s="4" t="s">
+      <c r="AO27" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="AQ27" s="3" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="28" spans="1:20" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="4">
-        <v>1</v>
-      </c>
-      <c r="B28" s="5" t="s">
+    <row r="28" spans="1:43" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>1</v>
+      </c>
+      <c r="B28" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="C28" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="L28" s="3">
+        <v>1206</v>
+      </c>
+      <c r="M28" s="3">
+        <v>0.03</v>
+      </c>
+      <c r="O28" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="P28" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="Q28" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="R28" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="X28" s="6">
+        <v>1</v>
+      </c>
+      <c r="Y28" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="Z28" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="D28" s="4" t="s">
+      <c r="AA28" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="E28" s="4" t="s">
+      <c r="AB28" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="M28" s="4">
+      <c r="AC28" s="6"/>
+      <c r="AD28" s="6"/>
+      <c r="AE28" s="6"/>
+      <c r="AF28" s="6"/>
+      <c r="AG28" s="6"/>
+      <c r="AH28" s="6"/>
+      <c r="AI28" s="6"/>
+      <c r="AJ28" s="3">
         <v>1206</v>
       </c>
-      <c r="N28" s="4">
+      <c r="AK28" s="3">
         <v>0.03</v>
       </c>
-      <c r="P28" s="9">
+      <c r="AM28" s="7">
         <v>0.01</v>
       </c>
-      <c r="R28" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="T28" s="4" t="s">
+      <c r="AO28" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="AQ28" s="3" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="29" spans="1:20" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="4">
-        <v>1</v>
-      </c>
-      <c r="B29" s="5" t="s">
+    <row r="29" spans="1:43" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>1</v>
+      </c>
+      <c r="B29" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="C29" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="L29" s="3">
+        <v>603</v>
+      </c>
+      <c r="M29" s="3">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="O29" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="P29" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q29" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="R29" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="X29" s="6">
+        <v>1</v>
+      </c>
+      <c r="Y29" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="Z29" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="D29" s="4" t="s">
+      <c r="AA29" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E29" s="4" t="s">
+      <c r="AB29" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="M29" s="4">
+      <c r="AC29" s="6"/>
+      <c r="AD29" s="6"/>
+      <c r="AE29" s="6"/>
+      <c r="AF29" s="6"/>
+      <c r="AG29" s="6"/>
+      <c r="AH29" s="6"/>
+      <c r="AI29" s="6"/>
+      <c r="AJ29" s="3">
         <v>603</v>
       </c>
-      <c r="N29" s="4">
+      <c r="AK29" s="3">
         <v>5.8999999999999997E-2</v>
       </c>
-      <c r="P29" s="9">
+      <c r="AM29" s="7">
         <v>0.01</v>
       </c>
-      <c r="R29" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="30" spans="1:20" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="4">
-        <v>1</v>
-      </c>
-      <c r="B30" s="5" t="s">
+      <c r="AO29" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="30" spans="1:43" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>1</v>
+      </c>
+      <c r="B30" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="C30" s="4" t="s">
+      <c r="C30" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="L30" s="3">
+        <v>603</v>
+      </c>
+      <c r="M30" s="3">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="O30" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="P30" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q30" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="R30" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="X30" s="6">
+        <v>1</v>
+      </c>
+      <c r="Y30" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="Z30" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="D30" s="4" t="s">
+      <c r="AA30" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E30" s="4" t="s">
+      <c r="AB30" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="M30" s="4">
+      <c r="AC30" s="6"/>
+      <c r="AD30" s="6"/>
+      <c r="AE30" s="6"/>
+      <c r="AF30" s="6"/>
+      <c r="AG30" s="6"/>
+      <c r="AH30" s="6"/>
+      <c r="AI30" s="6"/>
+      <c r="AJ30" s="3">
         <v>603</v>
       </c>
-      <c r="N30" s="4">
+      <c r="AK30" s="3">
         <v>5.8999999999999997E-2</v>
       </c>
-      <c r="P30" s="9">
+      <c r="AM30" s="7">
         <v>0.01</v>
       </c>
-      <c r="R30" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="T30" s="4" t="s">
+      <c r="AO30" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="AQ30" s="3" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="31" spans="1:20" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="4">
+    <row r="31" spans="1:43" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31">
         <v>2</v>
       </c>
-      <c r="B31" s="5" t="s">
+      <c r="B31" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="C31" s="4" t="s">
+      <c r="C31" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="L31" s="3">
+        <v>603</v>
+      </c>
+      <c r="M31" s="3">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="O31" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="P31" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q31" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="R31" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="X31" s="6">
+        <v>2</v>
+      </c>
+      <c r="Y31" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="Z31" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="D31" s="4" t="s">
+      <c r="AA31" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E31" s="4" t="s">
+      <c r="AB31" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="M31" s="4">
+      <c r="AC31" s="6"/>
+      <c r="AD31" s="6"/>
+      <c r="AE31" s="6"/>
+      <c r="AF31" s="6"/>
+      <c r="AG31" s="6"/>
+      <c r="AH31" s="6"/>
+      <c r="AI31" s="6"/>
+      <c r="AJ31" s="3">
         <v>603</v>
       </c>
-      <c r="N31" s="4">
+      <c r="AK31" s="3">
         <v>5.8999999999999997E-2</v>
       </c>
-      <c r="P31" s="9">
+      <c r="AM31" s="7">
         <v>0.01</v>
       </c>
-      <c r="R31" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="T31" s="4" t="s">
+      <c r="AO31" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="AQ31" s="3" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="32" spans="1:20" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="4">
+    <row r="32" spans="1:43" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32">
         <v>2</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="B32" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="C32" s="4" t="s">
+      <c r="C32" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="D32" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="D32" s="4" t="s">
+      <c r="J32" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="K32" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="T32" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="V32" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="X32" s="6">
+        <v>2</v>
+      </c>
+      <c r="Y32" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="Z32" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="AA32" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="E32" s="4" t="s">
+      <c r="AB32" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="K32" s="4" t="s">
+      <c r="AC32" s="6"/>
+      <c r="AD32" s="6"/>
+      <c r="AE32" s="6"/>
+      <c r="AF32" s="6"/>
+      <c r="AG32" s="6"/>
+      <c r="AH32" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="L32" s="4" t="s">
+      <c r="AI32" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="R32" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="33" spans="1:20" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="4">
-        <v>1</v>
-      </c>
-      <c r="B33" s="5" t="s">
+      <c r="AO32" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="33" spans="1:43" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>1</v>
+      </c>
+      <c r="B33" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="C33" s="4" t="s">
+      <c r="C33" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="D33" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="D33" s="4" t="s">
+      <c r="J33" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="K33" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="M33" s="3">
+        <v>5.45</v>
+      </c>
+      <c r="T33" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="V33" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="X33" s="6">
+        <v>1</v>
+      </c>
+      <c r="Y33" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="Z33" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="AA33" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="E33" s="4" t="s">
+      <c r="AB33" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="K33" s="4" t="s">
+      <c r="AC33" s="6"/>
+      <c r="AD33" s="6"/>
+      <c r="AE33" s="6"/>
+      <c r="AF33" s="6"/>
+      <c r="AG33" s="6"/>
+      <c r="AH33" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="L33" s="4" t="s">
+      <c r="AI33" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="N33" s="4">
+      <c r="AK33" s="3">
         <v>5.45</v>
       </c>
-      <c r="R33" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="T33" s="4" t="s">
+      <c r="AO33" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="AQ33" s="3" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="34" spans="1:20" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="4">
-        <v>1</v>
-      </c>
-      <c r="B34" s="5" t="s">
+    <row r="34" spans="1:43" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>1</v>
+      </c>
+      <c r="B34" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="C34" s="4" t="s">
+      <c r="C34" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="D34" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="D34" s="4" t="s">
+      <c r="J34" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="K34" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="M34" s="3">
+        <v>6.25</v>
+      </c>
+      <c r="P34" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="E34" s="4" t="s">
+      <c r="Q34" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="T34" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="V34" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="X34" s="6">
+        <v>1</v>
+      </c>
+      <c r="Y34" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="Z34" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="K34" s="4" t="s">
+      <c r="AA34" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="AB34" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="AC34" s="6"/>
+      <c r="AD34" s="6"/>
+      <c r="AE34" s="6"/>
+      <c r="AF34" s="6"/>
+      <c r="AG34" s="6"/>
+      <c r="AH34" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="L34" s="4" t="s">
+      <c r="AI34" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="N34" s="4">
+      <c r="AK34" s="3">
         <v>6.25</v>
       </c>
-      <c r="R34" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="T34" s="4" t="s">
+      <c r="AO34" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="AQ34" s="3" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="35" spans="1:20" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="4">
-        <v>1</v>
-      </c>
-      <c r="B35" s="5" t="s">
+    <row r="35" spans="1:43" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>1</v>
+      </c>
+      <c r="B35" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="C35" s="4" t="s">
+      <c r="C35" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="D35" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="D35" s="4" t="s">
+      <c r="J35" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="K35" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="M35" s="3">
+        <v>1.83</v>
+      </c>
+      <c r="T35" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="V35" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="X35" s="6">
+        <v>1</v>
+      </c>
+      <c r="Y35" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="Z35" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="AA35" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="E35" s="4" t="s">
+      <c r="AB35" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="K35" s="4" t="s">
+      <c r="AC35" s="6"/>
+      <c r="AD35" s="6"/>
+      <c r="AE35" s="6"/>
+      <c r="AF35" s="6"/>
+      <c r="AG35" s="6"/>
+      <c r="AH35" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="L35" s="4" t="s">
+      <c r="AI35" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="N35" s="4">
+      <c r="AK35" s="3">
         <v>1.83</v>
       </c>
-      <c r="R35" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="T35" s="4" t="s">
+      <c r="AO35" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="AQ35" s="3" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="36" spans="1:20" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="4">
-        <v>1</v>
-      </c>
-      <c r="B36" s="5" t="s">
+    <row r="36" spans="1:43" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>1</v>
+      </c>
+      <c r="B36" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="C36" s="4" t="s">
+      <c r="C36" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="D36" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="D36" s="4" t="s">
+      <c r="J36" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="K36" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="M36" s="3">
+        <v>45.88</v>
+      </c>
+      <c r="T36" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="V36" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="X36" s="6">
+        <v>1</v>
+      </c>
+      <c r="Y36" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="Z36" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="AA36" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="E36" s="4" t="s">
+      <c r="AB36" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="K36" s="4" t="s">
+      <c r="AC36" s="6"/>
+      <c r="AD36" s="6"/>
+      <c r="AE36" s="6"/>
+      <c r="AF36" s="6"/>
+      <c r="AG36" s="6"/>
+      <c r="AH36" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="L36" s="4" t="s">
+      <c r="AI36" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="N36" s="4">
+      <c r="AK36" s="3">
         <v>45.88</v>
       </c>
-      <c r="R36" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="T36" s="4" t="s">
+      <c r="AO36" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="AQ36" s="3" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="37" spans="1:20" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="4">
-        <v>1</v>
-      </c>
-      <c r="B37" s="5" t="s">
+    <row r="37" spans="1:43" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>1</v>
+      </c>
+      <c r="B37" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="C37" s="4" t="s">
+      <c r="C37" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D37" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="D37" s="4" t="s">
+      <c r="J37" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="K37" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="M37" s="3">
+        <v>0.73</v>
+      </c>
+      <c r="T37" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="V37" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="X37" s="6">
+        <v>1</v>
+      </c>
+      <c r="Y37" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="Z37" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="AA37" s="6" t="s">
         <v>150</v>
       </c>
-      <c r="E37" s="4" t="s">
+      <c r="AB37" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="K37" s="4" t="s">
+      <c r="AC37" s="6"/>
+      <c r="AD37" s="6"/>
+      <c r="AE37" s="6"/>
+      <c r="AF37" s="6"/>
+      <c r="AG37" s="6"/>
+      <c r="AH37" s="6" t="s">
         <v>151</v>
       </c>
-      <c r="L37" s="4" t="s">
+      <c r="AI37" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="N37" s="4">
+      <c r="AK37" s="3">
         <v>0.73</v>
       </c>
-      <c r="R37" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="T37" s="4" t="s">
+      <c r="AO37" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="AQ37" s="3" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="38" spans="1:20" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="4">
-        <v>1</v>
-      </c>
-      <c r="B38" s="5" t="s">
+    <row r="38" spans="1:43" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>1</v>
+      </c>
+      <c r="B38" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="C38" s="4" t="s">
+      <c r="C38" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D38" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="D38" s="4" t="s">
+      <c r="J38" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="K38" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="M38" s="3">
+        <v>4.79</v>
+      </c>
+      <c r="T38" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="V38" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="X38" s="6">
+        <v>1</v>
+      </c>
+      <c r="Y38" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="Z38" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="AA38" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="E38" s="4" t="s">
+      <c r="AB38" s="6" t="s">
         <v>155</v>
       </c>
-      <c r="K38" s="4" t="s">
+      <c r="AC38" s="6"/>
+      <c r="AD38" s="6"/>
+      <c r="AE38" s="6"/>
+      <c r="AF38" s="6"/>
+      <c r="AG38" s="6"/>
+      <c r="AH38" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="L38" s="4" t="s">
+      <c r="AI38" s="6" t="s">
         <v>158</v>
       </c>
-      <c r="N38" s="4">
+      <c r="AK38" s="3">
         <v>4.79</v>
       </c>
-      <c r="R38" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="T38" s="4" t="s">
+      <c r="AO38" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="AQ38" s="3" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="39" spans="1:20" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="4">
-        <v>1</v>
-      </c>
-      <c r="B39" s="5" t="s">
+    <row r="39" spans="1:43" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>1</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="J39" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="K39" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="M39" s="3">
+        <v>0.53</v>
+      </c>
+      <c r="T39" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="V39" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="X39" s="6"/>
+      <c r="Y39" s="8"/>
+      <c r="Z39" s="6"/>
+      <c r="AA39" s="6"/>
+      <c r="AB39" s="6"/>
+      <c r="AC39" s="6"/>
+      <c r="AD39" s="6"/>
+      <c r="AE39" s="6"/>
+      <c r="AF39" s="6"/>
+      <c r="AG39" s="6"/>
+      <c r="AH39" s="6"/>
+      <c r="AI39" s="6"/>
+    </row>
+    <row r="40" spans="1:43" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>1</v>
+      </c>
+      <c r="B40" t="s">
         <v>160</v>
       </c>
-      <c r="C39" s="4" t="s">
+      <c r="C40" t="s">
+        <v>162</v>
+      </c>
+      <c r="D40" t="s">
         <v>161</v>
       </c>
-      <c r="D39" s="4" t="s">
+      <c r="E40"/>
+      <c r="F40"/>
+      <c r="G40"/>
+      <c r="H40"/>
+      <c r="I40"/>
+      <c r="J40" t="s">
+        <v>163</v>
+      </c>
+      <c r="K40" t="s">
+        <v>164</v>
+      </c>
+      <c r="L40"/>
+      <c r="M40">
+        <v>0.76</v>
+      </c>
+      <c r="N40"/>
+      <c r="O40"/>
+      <c r="P40"/>
+      <c r="Q40"/>
+      <c r="R40"/>
+      <c r="S40" t="s">
+        <v>165</v>
+      </c>
+      <c r="T40" t="s">
+        <v>46</v>
+      </c>
+      <c r="U40"/>
+      <c r="V40" t="s">
+        <v>166</v>
+      </c>
+      <c r="W40"/>
+      <c r="X40" s="6">
+        <v>1</v>
+      </c>
+      <c r="Y40" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="Z40" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="AA40" s="6" t="s">
         <v>162</v>
       </c>
-      <c r="E39" s="4" t="s">
+      <c r="AB40" s="6" t="s">
         <v>161</v>
       </c>
-      <c r="K39" s="4" t="s">
+      <c r="AC40" s="6"/>
+      <c r="AD40" s="6"/>
+      <c r="AE40" s="6"/>
+      <c r="AF40" s="6"/>
+      <c r="AG40" s="6"/>
+      <c r="AH40" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="L39" s="4" t="s">
+      <c r="AI40" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="N39" s="4">
+      <c r="AK40" s="3">
         <v>0.76</v>
       </c>
-      <c r="Q39" s="4" t="s">
+      <c r="AN40" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="R39" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="T39" s="4" t="s">
+      <c r="AO40" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="AQ40" s="3" t="s">
         <v>166</v>
       </c>
+    </row>
+    <row r="41" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="X41" s="4"/>
+      <c r="Y41" s="5"/>
+      <c r="Z41" s="4"/>
+      <c r="AA41" s="4"/>
+      <c r="AB41" s="4"/>
+      <c r="AC41" s="4"/>
+      <c r="AD41" s="4"/>
+      <c r="AE41" s="4"/>
+      <c r="AF41" s="4"/>
+      <c r="AG41" s="4"/>
+      <c r="AH41" s="4"/>
+      <c r="AI41" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>